<commit_message>
debugging and loading data
</commit_message>
<xml_diff>
--- a/0 - Field Data Sheets/Weir Calibration Field Form 2019 CURRENT 06_30_2019.xlsx
+++ b/0 - Field Data Sheets/Weir Calibration Field Form 2019 CURRENT 06_30_2019.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex.messina\Documents\GitHub\SD_County_LowFlow\0 - Field Data Sheets\for processing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex.messina\Documents\GitHub\SD_County_LowFlow\0 - Field Data Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
     <sheet name="ESRI_MAPINFO_SHEET" sheetId="3" state="veryHidden" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Form Responses 1'!$A$1:$U$231</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Form Responses 1'!$A$1:$U$350</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -1995,14 +1995,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:U350"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A271" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J318" sqref="J318"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G348" sqref="G348"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2013,7 +2013,7 @@
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
     <col min="6" max="6" width="51.33203125" style="17" customWidth="1"/>
-    <col min="7" max="7" width="7.77734375" customWidth="1"/>
+    <col min="7" max="7" width="35" customWidth="1"/>
     <col min="8" max="8" width="23.6640625" customWidth="1"/>
     <col min="9" max="9" width="5.88671875" customWidth="1"/>
     <col min="10" max="10" width="19.33203125" customWidth="1"/>
@@ -2076,7 +2076,7 @@
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
     </row>
-    <row r="2" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>43588.755538854166</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>3050</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>43588.760185335646</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>43588.762669606484</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>5900</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>43591.435261481485</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>43591.44535303241</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>11400</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>43591.464841817127</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>5200</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>43591.470591574078</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>43591.472597476852</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>43591.479208553239</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>5600</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>43591.485304733797</v>
       </c>
@@ -2387,7 +2387,7 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>43591.492769594908</v>
       </c>
@@ -2419,7 +2419,7 @@
         <v>8200</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>43591.502019652777</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>43591.512494085648</v>
       </c>
@@ -2483,7 +2483,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>43591.521164178237</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>43591.527513136578</v>
       </c>
@@ -2547,7 +2547,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>43591.537957824075</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>43591.548731967589</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>43591.560089768522</v>
       </c>
@@ -2643,7 +2643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>43591.572355104166</v>
       </c>
@@ -2672,7 +2672,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>43591.577724270828</v>
       </c>
@@ -2704,7 +2704,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>43591.58141392361</v>
       </c>
@@ -2736,7 +2736,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>43591.583598541663</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>43591.6724153588</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>43591.674202650465</v>
       </c>
@@ -2814,7 +2814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>43591.704277094905</v>
       </c>
@@ -2834,7 +2834,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>43591.755216921301</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>43591.757524560184</v>
       </c>
@@ -2874,7 +2874,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>43591.775486631945</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>43591.776427210643</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>43592.481644421292</v>
       </c>
@@ -2946,7 +2946,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>43592.482017627313</v>
       </c>
@@ -2975,7 +2975,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>43592.50501202546</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>43592.532280358791</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>43592.545401550931</v>
       </c>
@@ -3080,7 +3080,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>43592.637291597217</v>
       </c>
@@ -3112,7 +3112,7 @@
         <v>14200</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>43592.563986909721</v>
       </c>
@@ -3156,7 +3156,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>43592.580991099538</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v>3100</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>43592.581140219903</v>
       </c>
@@ -3232,7 +3232,7 @@
         <v>4480</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <v>43592.640366712963</v>
       </c>
@@ -3264,7 +3264,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>43592.657211875005</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>4090</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>43592.681611643522</v>
       </c>
@@ -3323,7 +3323,7 @@
       </c>
       <c r="J42" s="5"/>
     </row>
-    <row r="43" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>43592.691540694446</v>
       </c>
@@ -3367,7 +3367,7 @@
         <v>2375</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>43592.702423842595</v>
       </c>
@@ -3443,7 +3443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>43593.44123866898</v>
       </c>
@@ -3472,7 +3472,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>43593.460052071758</v>
       </c>
@@ -3516,7 +3516,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
         <v>43593.476238275463</v>
       </c>
@@ -3560,7 +3560,7 @@
         <v>1740</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>43593.518983738424</v>
       </c>
@@ -3604,7 +3604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <v>43593.527186284722</v>
       </c>
@@ -3633,7 +3633,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>43593.548600451388</v>
       </c>
@@ -3662,7 +3662,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <v>43593.553772789353</v>
       </c>
@@ -3706,7 +3706,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
         <v>43593.598725358795</v>
       </c>
@@ -3729,7 +3729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <v>43593.610852187499</v>
       </c>
@@ -3770,7 +3770,7 @@
         <v>6250</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <v>43593.612856157408</v>
       </c>
@@ -3811,7 +3811,7 @@
         <v>7580</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
         <v>43593.617690162035</v>
       </c>
@@ -3852,7 +3852,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="57" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
         <v>43593.618488009262</v>
       </c>
@@ -3875,7 +3875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
         <v>43593.619830208336</v>
       </c>
@@ -3916,7 +3916,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
         <v>43593.656584456017</v>
       </c>
@@ -3957,7 +3957,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="60" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
         <v>43593.658092847225</v>
       </c>
@@ -4001,7 +4001,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="61" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7">
         <v>43593.660192870375</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
         <v>43593.6652215625</v>
       </c>
@@ -4089,7 +4089,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
         <v>43593.691000405088</v>
       </c>
@@ -4109,7 +4109,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
         <v>43594.407145740741</v>
       </c>
@@ -4153,7 +4153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7">
         <v>43594.410411932869</v>
       </c>
@@ -4197,7 +4197,7 @@
         <v>2170</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="7">
         <v>43594.419389386574</v>
       </c>
@@ -4241,7 +4241,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <v>43594.424918101853</v>
       </c>
@@ -4285,7 +4285,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="7">
         <v>43594.431594340276</v>
       </c>
@@ -4317,7 +4317,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="7">
         <v>43594.432673472227</v>
       </c>
@@ -4361,7 +4361,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="7">
         <v>43594.435762604167</v>
       </c>
@@ -4405,7 +4405,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="7">
         <v>43594.444414444442</v>
       </c>
@@ -4449,7 +4449,7 @@
         <v>2460</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="7">
         <v>43594.445713379631</v>
       </c>
@@ -4481,7 +4481,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="7">
         <v>43594.461393437501</v>
       </c>
@@ -4513,7 +4513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="7">
         <v>43594.467428356482</v>
       </c>
@@ -4557,7 +4557,7 @@
         <v>5570</v>
       </c>
     </row>
-    <row r="75" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="7">
         <v>43594.491857604167</v>
       </c>
@@ -4601,7 +4601,7 @@
         <v>4680</v>
       </c>
     </row>
-    <row r="76" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="7">
         <v>43594.514163171298</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="77" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="7">
         <v>43594.530017488425</v>
       </c>
@@ -4671,7 +4671,7 @@
         <v>2670</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="7">
         <v>43594.584730694449</v>
       </c>
@@ -4694,7 +4694,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="7">
         <v>43594.611498634258</v>
       </c>
@@ -4720,7 +4720,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="7">
         <v>43594.624838090276</v>
       </c>
@@ -4764,7 +4764,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="7">
         <v>43594.648807557867</v>
       </c>
@@ -4808,7 +4808,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="82" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="7">
         <v>43594.653585208333</v>
       </c>
@@ -4831,7 +4831,7 @@
         <v>-2.6</v>
       </c>
     </row>
-    <row r="83" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="7">
         <v>43594.667883368056</v>
       </c>
@@ -4857,7 +4857,7 @@
         <v>-1.4</v>
       </c>
     </row>
-    <row r="84" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="7">
         <v>43594.676933946757</v>
       </c>
@@ -4877,7 +4877,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="85" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="7">
         <v>43594.68904351852</v>
       </c>
@@ -4921,7 +4921,7 @@
         <v>3890</v>
       </c>
     </row>
-    <row r="86" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="7">
         <v>43594.893515358795</v>
       </c>
@@ -4965,7 +4965,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="87" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="7">
         <v>43594.895805115739</v>
       </c>
@@ -5009,7 +5009,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="88" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="7">
         <v>43594.896885995375</v>
       </c>
@@ -5053,7 +5053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="7">
         <v>43594.89877886574</v>
       </c>
@@ -5097,7 +5097,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="90" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="7">
         <v>43594.900322071757</v>
       </c>
@@ -5138,7 +5138,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="91" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="7">
         <v>43594.901593657407</v>
       </c>
@@ -5179,7 +5179,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="92" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="7">
         <v>43594.903644548613</v>
       </c>
@@ -5220,7 +5220,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="93" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="7">
         <v>43594.905283796295</v>
       </c>
@@ -5305,7 +5305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="7">
         <v>43594.908273356486</v>
       </c>
@@ -5346,7 +5346,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="96" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="7">
         <v>43594.909638333338</v>
       </c>
@@ -5387,7 +5387,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="97" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="7">
         <v>43594.91069650463</v>
       </c>
@@ -5428,7 +5428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="7">
         <v>43594.912148344913</v>
       </c>
@@ -5469,7 +5469,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="99" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="7">
         <v>43594.913895949074</v>
       </c>
@@ -5510,7 +5510,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="100" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="7">
         <v>43595.442240902776</v>
       </c>
@@ -5530,7 +5530,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="101" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="7">
         <v>43595.448872152774</v>
       </c>
@@ -5571,7 +5571,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="102" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="7">
         <v>43595.470052662036</v>
       </c>
@@ -5606,7 +5606,7 @@
         <v>6300</v>
       </c>
     </row>
-    <row r="103" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="7">
         <v>43595.470242951385</v>
       </c>
@@ -5632,7 +5632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="7">
         <v>43595.472295949075</v>
       </c>
@@ -5676,7 +5676,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="105" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="7">
         <v>43595.474870532409</v>
       </c>
@@ -5720,7 +5720,7 @@
         <v>2980</v>
       </c>
     </row>
-    <row r="106" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="7">
         <v>43595.481380717596</v>
       </c>
@@ -5755,7 +5755,7 @@
         <v>7030</v>
       </c>
     </row>
-    <row r="107" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="7">
         <v>43595.490416296292</v>
       </c>
@@ -5796,7 +5796,7 @@
         <v>6300</v>
       </c>
     </row>
-    <row r="108" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="7">
         <v>43595.500877777777</v>
       </c>
@@ -5834,7 +5834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="7">
         <v>43595.509428749996</v>
       </c>
@@ -5869,7 +5869,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="110" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="7">
         <v>43595.513097534727</v>
       </c>
@@ -5913,7 +5913,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="111" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="7">
         <v>43595.516432615739</v>
       </c>
@@ -5954,7 +5954,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="112" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="7">
         <v>43595.524782893517</v>
       </c>
@@ -5998,7 +5998,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="113" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="7">
         <v>43595.537118668981</v>
       </c>
@@ -6042,7 +6042,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="114" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="7">
         <v>43595.554605081023</v>
       </c>
@@ -6065,7 +6065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="7">
         <v>43595.554936168977</v>
       </c>
@@ -6088,7 +6088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="7">
         <v>43595.556602696757</v>
       </c>
@@ -6111,7 +6111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="7">
         <v>43595.5592850463</v>
       </c>
@@ -6134,7 +6134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="7">
         <v>43595.568305081018</v>
       </c>
@@ -6169,7 +6169,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="119" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="7">
         <v>43595.569374467595</v>
       </c>
@@ -6210,7 +6210,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="120" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="7">
         <v>43595.586062511575</v>
       </c>
@@ -6245,7 +6245,7 @@
         <v>2650</v>
       </c>
     </row>
-    <row r="121" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="7">
         <v>43595.587130358792</v>
       </c>
@@ -6280,7 +6280,7 @@
         <v>2430</v>
       </c>
     </row>
-    <row r="122" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="7">
         <v>43595.588972465281</v>
       </c>
@@ -6315,7 +6315,7 @@
         <v>2430</v>
       </c>
     </row>
-    <row r="123" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="7">
         <v>43595.590072256949</v>
       </c>
@@ -6350,7 +6350,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="124" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="7">
         <v>43595.594992129627</v>
       </c>
@@ -6394,7 +6394,7 @@
         <v>1230</v>
       </c>
     </row>
-    <row r="125" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="7">
         <v>43595.619344803243</v>
       </c>
@@ -6438,7 +6438,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="126" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="7">
         <v>43595.663596446757</v>
       </c>
@@ -6473,7 +6473,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="127" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="7">
         <v>43595.682554699073</v>
       </c>
@@ -6514,7 +6514,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="128" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="7">
         <v>43595.689118402777</v>
       </c>
@@ -6549,7 +6549,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="129" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="7">
         <v>43595.691901261569</v>
       </c>
@@ -6569,7 +6569,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="130" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="7">
         <v>43595.693264699075</v>
       </c>
@@ -6592,7 +6592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="7">
         <v>43595.707292939813</v>
       </c>
@@ -6615,7 +6615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="7">
         <v>43595.708949965279</v>
       </c>
@@ -6638,7 +6638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="7">
         <v>43595.711790578702</v>
       </c>
@@ -6661,7 +6661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="7">
         <v>43595.725159085647</v>
       </c>
@@ -6684,7 +6684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="7">
         <v>43598.523171504625</v>
       </c>
@@ -6728,7 +6728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="7">
         <v>43598.531430370371</v>
       </c>
@@ -6772,7 +6772,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="137" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="7">
         <v>43598.538723784717</v>
       </c>
@@ -6816,7 +6816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="7">
         <v>43598.55321135417</v>
       </c>
@@ -6860,7 +6860,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="139" spans="1:15" s="11" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15" s="11" customFormat="1" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="10">
         <v>43598.558324872683</v>
       </c>
@@ -6889,7 +6889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="7">
         <v>43598.568272129633</v>
       </c>
@@ -6933,7 +6933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="7">
         <v>43598.660832187496</v>
       </c>
@@ -7009,7 +7009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="7">
         <v>43599.412810810187</v>
       </c>
@@ -7050,7 +7050,7 @@
         <v>3260</v>
       </c>
     </row>
-    <row r="144" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="7">
         <v>43599.427670717589</v>
       </c>
@@ -7094,7 +7094,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="145" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="7">
         <v>43599.433456574072</v>
       </c>
@@ -7138,7 +7138,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="146" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="7">
         <v>43599.459267349535</v>
       </c>
@@ -7182,7 +7182,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="147" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="7">
         <v>43599.470011574071</v>
       </c>
@@ -7226,7 +7226,7 @@
         <v>2520</v>
       </c>
     </row>
-    <row r="148" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="7">
         <v>43599.485035810183</v>
       </c>
@@ -7252,7 +7252,7 @@
         <v>16.8</v>
       </c>
     </row>
-    <row r="149" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="7">
         <v>43599.500831736106</v>
       </c>
@@ -7278,7 +7278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="7">
         <v>43599.518437384264</v>
       </c>
@@ -7304,7 +7304,7 @@
         <v>-2.7</v>
       </c>
     </row>
-    <row r="151" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="7">
         <v>43599.539609108797</v>
       </c>
@@ -7348,7 +7348,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="152" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="7">
         <v>43599.569834490743</v>
       </c>
@@ -7392,7 +7392,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="153" spans="1:15" s="11" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:15" s="11" customFormat="1" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="10">
         <v>43599.624617476853</v>
       </c>
@@ -7421,7 +7421,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="154" spans="1:15" s="11" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:15" s="11" customFormat="1" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="10">
         <v>43599.639232141199</v>
       </c>
@@ -7453,7 +7453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="7">
         <v>43599.738793206023</v>
       </c>
@@ -7497,7 +7497,7 @@
         <v>2160</v>
       </c>
     </row>
-    <row r="156" spans="1:15" s="11" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:15" s="11" customFormat="1" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="10">
         <v>43600.422265266199</v>
       </c>
@@ -7529,7 +7529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="7">
         <v>43600.482206006942</v>
       </c>
@@ -7573,7 +7573,7 @@
         <v>3240</v>
       </c>
     </row>
-    <row r="158" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="7">
         <v>43600.493555451394</v>
       </c>
@@ -7605,7 +7605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="7">
         <v>43600.498960439814</v>
       </c>
@@ -7649,7 +7649,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="160" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="7">
         <v>43600.528849884256</v>
       </c>
@@ -7693,7 +7693,7 @@
         <v>1450</v>
       </c>
     </row>
-    <row r="161" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="7">
         <v>43600.601932974532</v>
       </c>
@@ -7737,7 +7737,7 @@
         <v>2190</v>
       </c>
     </row>
-    <row r="162" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="7">
         <v>43600.638289583338</v>
       </c>
@@ -7781,7 +7781,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="163" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="7">
         <v>43600.686218657407</v>
       </c>
@@ -7825,7 +7825,7 @@
         <v>9850</v>
       </c>
     </row>
-    <row r="164" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="7">
         <v>43600.725389861109</v>
       </c>
@@ -7904,7 +7904,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="166" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="7">
         <v>43601.40923740741</v>
       </c>
@@ -7927,7 +7927,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="167" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="7">
         <v>43601.414449374999</v>
       </c>
@@ -7950,7 +7950,7 @@
         <v>-1.3</v>
       </c>
     </row>
-    <row r="168" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="7">
         <v>43601.415471493056</v>
       </c>
@@ -7979,7 +7979,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="169" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="7">
         <v>43601.417819421295</v>
       </c>
@@ -8008,7 +8008,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="170" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="7">
         <v>43601.419731273148</v>
       </c>
@@ -8037,7 +8037,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="171" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="7">
         <v>43601.427588611114</v>
       </c>
@@ -8066,7 +8066,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="172" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="7">
         <v>43602.442062349539</v>
       </c>
@@ -8139,7 +8139,7 @@
         <v>1190</v>
       </c>
     </row>
-    <row r="174" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="7">
         <v>43602.47989505787</v>
       </c>
@@ -8165,7 +8165,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="175" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="7">
         <v>43602.489967141199</v>
       </c>
@@ -8203,7 +8203,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="176" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="7">
         <v>43602.509337268522</v>
       </c>
@@ -8241,7 +8241,7 @@
         <v>3700</v>
       </c>
     </row>
-    <row r="177" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="7">
         <v>43602.522517500001</v>
       </c>
@@ -8276,7 +8276,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="178" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="7">
         <v>43606.707793877315</v>
       </c>
@@ -8317,7 +8317,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="179" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="7">
         <v>43606.723546145833</v>
       </c>
@@ -8358,7 +8358,7 @@
         <v>1830</v>
       </c>
     </row>
-    <row r="180" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="7">
         <v>43608.481453252316</v>
       </c>
@@ -8387,7 +8387,7 @@
         <v>9100</v>
       </c>
     </row>
-    <row r="181" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="7">
         <v>43608.482445162037</v>
       </c>
@@ -8416,7 +8416,7 @@
         <v>8050</v>
       </c>
     </row>
-    <row r="182" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="7">
         <v>43608.483487696758</v>
       </c>
@@ -8445,7 +8445,7 @@
         <v>7240</v>
       </c>
     </row>
-    <row r="183" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:15" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="7">
         <v>43608.526771817131</v>
       </c>
@@ -8477,7 +8477,7 @@
         <v>3480</v>
       </c>
     </row>
-    <row r="184" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="7">
         <v>43619.387044270828</v>
       </c>
@@ -8500,7 +8500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="7">
         <v>43619.417066539347</v>
       </c>
@@ -8529,7 +8529,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="186" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="7">
         <v>43619.424325891203</v>
       </c>
@@ -8564,7 +8564,7 @@
         <v>8600</v>
       </c>
     </row>
-    <row r="187" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="7">
         <v>43619.430370590278</v>
       </c>
@@ -8593,7 +8593,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="188" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="7">
         <v>43619.448148344905</v>
       </c>
@@ -8616,7 +8616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="7">
         <v>43619.449386782406</v>
       </c>
@@ -8660,7 +8660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="7">
         <v>43619.457925891205</v>
       </c>
@@ -8704,7 +8704,7 @@
         <v>4910</v>
       </c>
     </row>
-    <row r="191" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="7">
         <v>43619.481042361112</v>
       </c>
@@ -8727,7 +8727,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="192" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="7">
         <v>43619.482240219906</v>
       </c>
@@ -8756,7 +8756,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="193" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="7">
         <v>43619.485708449072</v>
       </c>
@@ -8785,7 +8785,7 @@
         <v>2470</v>
       </c>
     </row>
-    <row r="194" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="7">
         <v>43619.502512523148</v>
       </c>
@@ -8814,7 +8814,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="195" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="7">
         <v>43619.50333712963</v>
       </c>
@@ -8837,7 +8837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="7">
         <v>43619.512569479164</v>
       </c>
@@ -8860,7 +8860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="7">
         <v>43619.559027557872</v>
       </c>
@@ -8883,7 +8883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="7">
         <v>43619.560911979162</v>
       </c>
@@ -8906,7 +8906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="7">
         <v>43619.580106157402</v>
       </c>
@@ -8935,7 +8935,7 @@
         <v>8500</v>
       </c>
     </row>
-    <row r="200" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="7">
         <v>43619.586162476851</v>
       </c>
@@ -8958,7 +8958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="7">
         <v>43619.593100185186</v>
       </c>
@@ -8990,7 +8990,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="202" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="7">
         <v>43619.603138240738</v>
       </c>
@@ -9019,7 +9019,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="203" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="7">
         <v>43619.624149479168</v>
       </c>
@@ -9048,7 +9048,7 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="204" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="7">
         <v>43619.636075578703</v>
       </c>
@@ -9080,7 +9080,7 @@
         <v>2820</v>
       </c>
     </row>
-    <row r="205" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="7">
         <v>43619.657319212958</v>
       </c>
@@ -9112,7 +9112,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="206" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="7">
         <v>43619.669281388888</v>
       </c>
@@ -9135,7 +9135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="7">
         <v>43619.683368090278</v>
       </c>
@@ -9167,7 +9167,7 @@
         <v>2220</v>
       </c>
     </row>
-    <row r="208" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="7">
         <v>43620.42668315972</v>
       </c>
@@ -9193,7 +9193,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="209" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="7">
         <v>43620.433715914347</v>
       </c>
@@ -9222,7 +9222,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="210" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="7">
         <v>43620.449795451394</v>
       </c>
@@ -9251,7 +9251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="7">
         <v>43620.468617280094</v>
       </c>
@@ -9295,7 +9295,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="212" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="7">
         <v>43620.486011516201</v>
       </c>
@@ -9336,7 +9336,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="213" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="7">
         <v>43620.487928645831</v>
       </c>
@@ -9365,7 +9365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="7">
         <v>43620.488378425929</v>
       </c>
@@ -9385,7 +9385,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="215" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="7">
         <v>43620.488762453708</v>
       </c>
@@ -9405,7 +9405,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="216" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="7">
         <v>43620.502757766204</v>
       </c>
@@ -9475,7 +9475,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="218" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="7">
         <v>43620.516394976847</v>
       </c>
@@ -9501,7 +9501,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="219" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="7">
         <v>43620.531383842594</v>
       </c>
@@ -9524,7 +9524,7 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="220" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="7">
         <v>43620.534318229169</v>
       </c>
@@ -9553,7 +9553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="7">
         <v>43620.53862825231</v>
       </c>
@@ -9582,7 +9582,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="222" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="7">
         <v>43620.544621446759</v>
       </c>
@@ -9605,7 +9605,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="223" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="7">
         <v>43620.559045000002</v>
       </c>
@@ -9646,7 +9646,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="224" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="7">
         <v>43620.562107916667</v>
       </c>
@@ -9669,7 +9669,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="225" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="7">
         <v>43620.57524528935</v>
       </c>
@@ -9710,7 +9710,7 @@
         <v>1540</v>
       </c>
     </row>
-    <row r="226" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="7">
         <v>43620.57848960648</v>
       </c>
@@ -9739,7 +9739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="7">
         <v>43620.589187465273</v>
       </c>
@@ -9762,7 +9762,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="228" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="7">
         <v>43620.646162557867</v>
       </c>
@@ -9803,7 +9803,7 @@
         <v>2215</v>
       </c>
     </row>
-    <row r="229" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="7">
         <v>43620.686772013883</v>
       </c>
@@ -9826,7 +9826,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="230" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="7">
         <v>43623.521720659723</v>
       </c>
@@ -9849,7 +9849,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="231" spans="1:15" s="22" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:15" s="22" customFormat="1" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="18">
         <v>43623.522309618056</v>
       </c>
@@ -9872,7 +9872,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="232" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="7">
         <v>43633.40398304398</v>
       </c>
@@ -9901,7 +9901,7 @@
         <v>5100</v>
       </c>
     </row>
-    <row r="233" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="7">
         <v>43633.416756932871</v>
       </c>
@@ -9930,7 +9930,7 @@
         <v>5100</v>
       </c>
     </row>
-    <row r="234" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="7">
         <v>43633.420208194446</v>
       </c>
@@ -9959,7 +9959,7 @@
         <v>14250</v>
       </c>
     </row>
-    <row r="235" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="7">
         <v>43633.428534791667</v>
       </c>
@@ -9988,7 +9988,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="236" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="7">
         <v>43633.4461915625</v>
       </c>
@@ -10017,7 +10017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="7">
         <v>43633.46175555556</v>
       </c>
@@ -10061,7 +10061,7 @@
         <v>2270</v>
       </c>
     </row>
-    <row r="238" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="7">
         <v>43633.50244113426</v>
       </c>
@@ -10090,7 +10090,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="239" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="7">
         <v>43633.504802060183</v>
       </c>
@@ -10119,7 +10119,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="240" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="7">
         <v>43633.523931469907</v>
       </c>
@@ -10148,7 +10148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="7">
         <v>43633.530496736115</v>
       </c>
@@ -10192,7 +10192,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="242" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="7">
         <v>43633.533061898153</v>
       </c>
@@ -10221,7 +10221,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="243" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="7">
         <v>43633.539491469906</v>
       </c>
@@ -10250,7 +10250,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="244" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="7">
         <v>43633.543584953703</v>
       </c>
@@ -10279,7 +10279,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="245" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="7">
         <v>43633.547313564814</v>
       </c>
@@ -10308,7 +10308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="7">
         <v>43633.551025127315</v>
       </c>
@@ -10337,7 +10337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="7">
         <v>43633.562344479171</v>
       </c>
@@ -10366,7 +10366,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="248" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="7">
         <v>43633.590683958333</v>
       </c>
@@ -10410,7 +10410,7 @@
         <v>9400</v>
       </c>
     </row>
-    <row r="249" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="7">
         <v>43633.581785532406</v>
       </c>
@@ -10439,7 +10439,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="250" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" s="7">
         <v>43633.625512199069</v>
       </c>
@@ -10465,7 +10465,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="251" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" s="7">
         <v>43633.627015150458</v>
       </c>
@@ -10494,7 +10494,7 @@
         <v>7400</v>
       </c>
     </row>
-    <row r="252" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="7">
         <v>43633.63865868056</v>
       </c>
@@ -10526,7 +10526,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="253" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="7">
         <v>43633.660197569443</v>
       </c>
@@ -10558,7 +10558,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="254" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" s="7">
         <v>43633.689922777776</v>
       </c>
@@ -10590,7 +10590,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="255" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" s="7">
         <v>43634.393672152779</v>
       </c>
@@ -10619,7 +10619,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="256" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" s="7">
         <v>43634.396875138889</v>
       </c>
@@ -10648,7 +10648,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="257" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" s="7">
         <v>43634.405545023154</v>
       </c>
@@ -10677,7 +10677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" s="7">
         <v>43634.416232280091</v>
       </c>
@@ -10706,7 +10706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="7">
         <v>43634.420364861115</v>
       </c>
@@ -10735,7 +10735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" s="7">
         <v>43634.424504351853</v>
       </c>
@@ -10779,7 +10779,7 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="261" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="7">
         <v>43634.427363206021</v>
       </c>
@@ -10808,7 +10808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" s="7">
         <v>43634.437920937504</v>
       </c>
@@ -10837,7 +10837,7 @@
         <v>7250</v>
       </c>
     </row>
-    <row r="263" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" s="7">
         <v>43634.446620960647</v>
       </c>
@@ -10866,7 +10866,7 @@
         <v>9500</v>
       </c>
     </row>
-    <row r="264" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" s="7">
         <v>43634.454626250001</v>
       </c>
@@ -10895,7 +10895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" s="7">
         <v>43634.456643518519</v>
       </c>
@@ -10927,7 +10927,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="266" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" s="7">
         <v>43634.458449259255</v>
       </c>
@@ -10956,7 +10956,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="267" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" s="7">
         <v>43634.469420011577</v>
       </c>
@@ -10985,7 +10985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" s="7">
         <v>43634.472232048611</v>
       </c>
@@ -11014,7 +11014,7 @@
         <v>3400</v>
       </c>
     </row>
-    <row r="269" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" s="7">
         <v>43634.478026145836</v>
       </c>
@@ -11043,7 +11043,7 @@
         <v>3150</v>
       </c>
     </row>
-    <row r="270" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" s="7">
         <v>43634.478377719905</v>
       </c>
@@ -11072,7 +11072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" s="7">
         <v>43634.486881469908</v>
       </c>
@@ -11101,7 +11101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" s="7">
         <v>43634.488325983795</v>
       </c>
@@ -11130,7 +11130,7 @@
         <v>8100</v>
       </c>
     </row>
-    <row r="273" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" s="7">
         <v>43634.496477800931</v>
       </c>
@@ -11162,7 +11162,7 @@
         <v>8100</v>
       </c>
     </row>
-    <row r="274" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" s="7">
         <v>43634.500037627316</v>
       </c>
@@ -11191,7 +11191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" s="7">
         <v>43634.503317557872</v>
       </c>
@@ -11220,7 +11220,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="276" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" s="7">
         <v>43634.5105887963</v>
       </c>
@@ -11249,7 +11249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" s="7">
         <v>43634.51392675926</v>
       </c>
@@ -11281,7 +11281,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="278" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" s="7">
         <v>43634.530469999998</v>
       </c>
@@ -11310,7 +11310,7 @@
         <v>1760</v>
       </c>
     </row>
-    <row r="279" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" s="7">
         <v>43634.56578636574</v>
       </c>
@@ -11400,7 +11400,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="282" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" s="7">
         <v>43634.633482164354</v>
       </c>
@@ -11429,7 +11429,7 @@
         <v>5100</v>
       </c>
     </row>
-    <row r="283" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" s="7">
         <v>43637.422400451389</v>
       </c>
@@ -11458,7 +11458,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="284" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" s="7">
         <v>43641.40604130787</v>
       </c>
@@ -11499,7 +11499,7 @@
         <v>3015</v>
       </c>
     </row>
-    <row r="285" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" s="7">
         <v>43641.415160428238</v>
       </c>
@@ -11540,7 +11540,7 @@
         <v>2750</v>
       </c>
     </row>
-    <row r="286" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" s="7">
         <v>43641.438067060182</v>
       </c>
@@ -11581,7 +11581,7 @@
         <v>2620</v>
       </c>
     </row>
-    <row r="287" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" s="7">
         <v>43641.454948587962</v>
       </c>
@@ -11622,7 +11622,7 @@
         <v>2475</v>
       </c>
     </row>
-    <row r="288" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" s="7">
         <v>43641.468790266204</v>
       </c>
@@ -11663,7 +11663,7 @@
         <v>2640</v>
       </c>
     </row>
-    <row r="289" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" s="7">
         <v>43641.543771076387</v>
       </c>
@@ -11704,7 +11704,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="290" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" s="7">
         <v>43641.555053761578</v>
       </c>
@@ -11745,7 +11745,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="291" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" s="7">
         <v>43641.635631805555</v>
       </c>
@@ -11786,7 +11786,7 @@
         <v>1815</v>
       </c>
     </row>
-    <row r="292" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" s="7">
         <v>43641.647440000001</v>
       </c>
@@ -11827,7 +11827,7 @@
         <v>1565</v>
       </c>
     </row>
-    <row r="293" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" s="7">
         <v>43641.6602040625</v>
       </c>
@@ -11868,7 +11868,7 @@
         <v>1645</v>
       </c>
     </row>
-    <row r="294" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" s="7">
         <v>43641.689663888887</v>
       </c>
@@ -11909,7 +11909,7 @@
         <v>1730</v>
       </c>
     </row>
-    <row r="295" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" s="7">
         <v>43641.701291400459</v>
       </c>
@@ -11950,7 +11950,7 @@
         <v>1930</v>
       </c>
     </row>
-    <row r="296" spans="1:17" s="22" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:17" s="22" customFormat="1" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" s="18">
         <v>43641.717524178239</v>
       </c>
@@ -11994,7 +11994,7 @@
         <v>2120</v>
       </c>
     </row>
-    <row r="297" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" s="7">
         <v>43647.378567395834</v>
       </c>
@@ -12027,7 +12027,7 @@
       </c>
       <c r="Q297" s="5"/>
     </row>
-    <row r="298" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" s="7">
         <v>43647.39412060185</v>
       </c>
@@ -12060,7 +12060,7 @@
       </c>
       <c r="Q298" s="5"/>
     </row>
-    <row r="299" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" s="7">
         <v>43647.403549803239</v>
       </c>
@@ -12093,7 +12093,7 @@
       </c>
       <c r="Q299" s="5"/>
     </row>
-    <row r="300" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" s="7">
         <v>43647.418112916668</v>
       </c>
@@ -12126,7 +12126,7 @@
       </c>
       <c r="Q300" s="5"/>
     </row>
-    <row r="301" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" s="7">
         <v>43647.437997430556</v>
       </c>
@@ -12158,7 +12158,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="302" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" s="7">
         <v>43647.442859641204</v>
       </c>
@@ -12191,7 +12191,7 @@
       </c>
       <c r="Q302" s="5"/>
     </row>
-    <row r="303" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" s="7">
         <v>43647.44526699074</v>
       </c>
@@ -12224,7 +12224,7 @@
       </c>
       <c r="Q303" s="5"/>
     </row>
-    <row r="304" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" s="7">
         <v>43647.445862928245</v>
       </c>
@@ -12257,7 +12257,7 @@
       </c>
       <c r="Q304" s="5"/>
     </row>
-    <row r="305" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" s="7">
         <v>43647.452365173609</v>
       </c>
@@ -12290,7 +12290,7 @@
       </c>
       <c r="Q305" s="5"/>
     </row>
-    <row r="306" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" s="7">
         <v>43647.46204752315</v>
       </c>
@@ -12323,7 +12323,7 @@
       </c>
       <c r="Q306" s="5"/>
     </row>
-    <row r="307" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" s="7">
         <v>43647.47148359954</v>
       </c>
@@ -12356,7 +12356,7 @@
       </c>
       <c r="Q307" s="5"/>
     </row>
-    <row r="308" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" s="7">
         <v>43647.475172638893</v>
       </c>
@@ -12389,7 +12389,7 @@
       </c>
       <c r="Q308" s="5"/>
     </row>
-    <row r="309" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" s="7">
         <v>43647.482570231485</v>
       </c>
@@ -12422,7 +12422,7 @@
       </c>
       <c r="Q309" s="5"/>
     </row>
-    <row r="310" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" s="7">
         <v>43647.489491956017</v>
       </c>
@@ -12455,7 +12455,7 @@
       </c>
       <c r="Q310" s="5"/>
     </row>
-    <row r="311" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" s="7">
         <v>43647.495944016206</v>
       </c>
@@ -12488,7 +12488,7 @@
       </c>
       <c r="Q311" s="5"/>
     </row>
-    <row r="312" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" s="7">
         <v>43647.496494571758</v>
       </c>
@@ -12521,7 +12521,7 @@
       </c>
       <c r="Q312" s="5"/>
     </row>
-    <row r="313" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" s="7">
         <v>43647.5053858912</v>
       </c>
@@ -12554,7 +12554,7 @@
       </c>
       <c r="Q313" s="5"/>
     </row>
-    <row r="314" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" s="7">
         <v>43647.512554305555</v>
       </c>
@@ -12590,7 +12590,7 @@
       </c>
       <c r="Q314" s="5"/>
     </row>
-    <row r="315" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" s="7">
         <v>43647.513685578699</v>
       </c>
@@ -12623,7 +12623,7 @@
       </c>
       <c r="Q315" s="5"/>
     </row>
-    <row r="316" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" s="7">
         <v>43647.518523483799</v>
       </c>
@@ -12656,7 +12656,7 @@
       </c>
       <c r="Q316" s="5"/>
     </row>
-    <row r="317" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" s="7">
         <v>43647.519861805558</v>
       </c>
@@ -12692,7 +12692,7 @@
       </c>
       <c r="Q317" s="5"/>
     </row>
-    <row r="318" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" s="7">
         <v>43647.535344895834</v>
       </c>
@@ -12725,7 +12725,7 @@
       </c>
       <c r="Q318" s="5"/>
     </row>
-    <row r="319" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" s="7">
         <v>43647.537166388887</v>
       </c>
@@ -12758,7 +12758,7 @@
       </c>
       <c r="Q319" s="5"/>
     </row>
-    <row r="320" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" s="7">
         <v>43647.538050277777</v>
       </c>
@@ -12791,7 +12791,7 @@
       </c>
       <c r="Q320" s="5"/>
     </row>
-    <row r="321" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" s="7">
         <v>43647.540616631944</v>
       </c>
@@ -12824,7 +12824,7 @@
       </c>
       <c r="Q321" s="5"/>
     </row>
-    <row r="322" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" s="7">
         <v>43647.54435773148</v>
       </c>
@@ -12857,7 +12857,7 @@
       </c>
       <c r="Q322" s="5"/>
     </row>
-    <row r="323" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" s="7">
         <v>43647.547887106484</v>
       </c>
@@ -12890,7 +12890,7 @@
       </c>
       <c r="Q323" s="5"/>
     </row>
-    <row r="324" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" s="7">
         <v>43647.551679976852</v>
       </c>
@@ -12923,7 +12923,7 @@
       </c>
       <c r="Q324" s="5"/>
     </row>
-    <row r="325" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" s="7">
         <v>43647.55485487268</v>
       </c>
@@ -12956,7 +12956,7 @@
       </c>
       <c r="Q325" s="5"/>
     </row>
-    <row r="326" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" s="7">
         <v>43647.586594768523</v>
       </c>
@@ -12992,7 +12992,7 @@
       </c>
       <c r="Q326" s="5"/>
     </row>
-    <row r="327" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" s="7">
         <v>43647.578063356486</v>
       </c>
@@ -13025,7 +13025,7 @@
       </c>
       <c r="Q327" s="5"/>
     </row>
-    <row r="328" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" s="7">
         <v>43647.581616527779</v>
       </c>
@@ -13061,7 +13061,7 @@
       </c>
       <c r="Q328" s="5"/>
     </row>
-    <row r="329" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" s="7">
         <v>43647.586999560182</v>
       </c>
@@ -13097,7 +13097,7 @@
       </c>
       <c r="Q329" s="5"/>
     </row>
-    <row r="330" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" s="7">
         <v>43647.587708356485</v>
       </c>
@@ -13130,7 +13130,7 @@
       </c>
       <c r="Q330" s="5"/>
     </row>
-    <row r="331" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" s="7">
         <v>43647.58930334491</v>
       </c>
@@ -13163,7 +13163,7 @@
       </c>
       <c r="Q331" s="5"/>
     </row>
-    <row r="332" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" s="7">
         <v>43647.614860520829</v>
       </c>
@@ -13196,7 +13196,7 @@
       </c>
       <c r="Q332" s="5"/>
     </row>
-    <row r="333" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" s="7">
         <v>43647.616616493055</v>
       </c>
@@ -13229,7 +13229,7 @@
       </c>
       <c r="Q333" s="5"/>
     </row>
-    <row r="334" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334" s="7">
         <v>43647.628458217594</v>
       </c>
@@ -13256,7 +13256,7 @@
       </c>
       <c r="Q334" s="5"/>
     </row>
-    <row r="335" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335" s="7">
         <v>43647.648176006944</v>
       </c>
@@ -13289,7 +13289,7 @@
       </c>
       <c r="Q335" s="5"/>
     </row>
-    <row r="336" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" s="7">
         <v>43647.652004189818</v>
       </c>
@@ -13322,7 +13322,7 @@
       </c>
       <c r="Q336" s="5"/>
     </row>
-    <row r="337" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" s="7">
         <v>43647.663755868052</v>
       </c>
@@ -13355,7 +13355,7 @@
       </c>
       <c r="Q337" s="5"/>
     </row>
-    <row r="338" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" s="7">
         <v>43648.434577314816</v>
       </c>
@@ -13391,7 +13391,7 @@
       </c>
       <c r="Q338" s="5"/>
     </row>
-    <row r="339" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339" s="7">
         <v>43648.464827615739</v>
       </c>
@@ -13424,7 +13424,7 @@
       </c>
       <c r="Q339" s="5"/>
     </row>
-    <row r="340" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340" s="7">
         <v>43648.49087303241</v>
       </c>
@@ -13454,7 +13454,7 @@
       </c>
       <c r="Q340" s="5"/>
     </row>
-    <row r="341" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341" s="7">
         <v>43648.505817361111</v>
       </c>
@@ -13487,7 +13487,7 @@
       </c>
       <c r="Q341" s="5"/>
     </row>
-    <row r="342" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342" s="7">
         <v>43648.523454918977</v>
       </c>
@@ -13517,7 +13517,7 @@
       </c>
       <c r="Q342" s="5"/>
     </row>
-    <row r="343" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343" s="7">
         <v>43648.535805590276</v>
       </c>
@@ -13543,7 +13543,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="344" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" s="7">
         <v>43648.557352407406</v>
       </c>
@@ -13576,7 +13576,7 @@
       </c>
       <c r="Q344" s="5"/>
     </row>
-    <row r="345" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" s="7">
         <v>43648.574154016205</v>
       </c>
@@ -13612,7 +13612,7 @@
       </c>
       <c r="Q345" s="5"/>
     </row>
-    <row r="346" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" s="7">
         <v>43648.597286747681</v>
       </c>
@@ -13645,7 +13645,7 @@
       </c>
       <c r="Q346" s="5"/>
     </row>
-    <row r="347" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347" s="7">
         <v>43648.600304039355</v>
       </c>
@@ -13714,7 +13714,7 @@
       </c>
       <c r="Q348" s="5"/>
     </row>
-    <row r="349" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" s="7">
         <v>43657.492113460648</v>
       </c>
@@ -13743,7 +13743,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="350" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" s="7">
         <v>43657.493938182874</v>
       </c>
@@ -13776,6 +13776,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:U350">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="SDG-072"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1"/>
     <hyperlink ref="G6" r:id="rId2"/>

</xml_diff>

<commit_message>
Alex finished his and committing
</commit_message>
<xml_diff>
--- a/0 - Field Data Sheets/Weir Calibration Field Form 2019 CURRENT 06_30_2019.xlsx
+++ b/0 - Field Data Sheets/Weir Calibration Field Form 2019 CURRENT 06_30_2019.xlsx
@@ -36,6 +36,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Responder updated this value.</t>
         </r>
@@ -48,6 +49,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Responder updated this value.</t>
         </r>
@@ -60,6 +62,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Responder updated this value.</t>
         </r>
@@ -72,6 +75,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Responder updated this value.</t>
         </r>
@@ -84,6 +88,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Responder updated this value.</t>
         </r>
@@ -1512,7 +1517,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1521,23 +1526,27 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1547,6 +1556,12 @@
     <font>
       <u/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1586,7 +1601,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1621,6 +1636,7 @@
     <xf numFmtId="19" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1995,14 +2011,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:U350"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G348" sqref="G348"/>
+      <selection pane="bottomLeft" activeCell="K136" sqref="K136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2011,9 +2027,9 @@
     <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="6" max="6" width="51.33203125" style="17" customWidth="1"/>
-    <col min="7" max="7" width="35" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" customWidth="1"/>
+    <col min="6" max="6" width="34.44140625" style="17" customWidth="1"/>
+    <col min="7" max="7" width="36.88671875" customWidth="1"/>
     <col min="8" max="8" width="23.6640625" customWidth="1"/>
     <col min="9" max="9" width="5.88671875" customWidth="1"/>
     <col min="10" max="10" width="19.33203125" customWidth="1"/>
@@ -2076,7 +2092,7 @@
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
     </row>
-    <row r="2" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>43588.755538854166</v>
       </c>
@@ -2105,7 +2121,7 @@
         <v>3050</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>43588.760185335646</v>
       </c>
@@ -2134,7 +2150,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>43588.762669606484</v>
       </c>
@@ -2163,7 +2179,7 @@
         <v>5900</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>43591.435261481485</v>
       </c>
@@ -2195,7 +2211,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>43591.44535303241</v>
       </c>
@@ -2227,7 +2243,7 @@
         <v>11400</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>43591.464841817127</v>
       </c>
@@ -2259,7 +2275,7 @@
         <v>5200</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>43591.470591574078</v>
       </c>
@@ -2291,7 +2307,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>43591.472597476852</v>
       </c>
@@ -2323,7 +2339,7 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>43591.479208553239</v>
       </c>
@@ -2355,7 +2371,7 @@
         <v>5600</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>43591.485304733797</v>
       </c>
@@ -2387,7 +2403,7 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>43591.492769594908</v>
       </c>
@@ -2419,7 +2435,7 @@
         <v>8200</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>43591.502019652777</v>
       </c>
@@ -2451,7 +2467,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>43591.512494085648</v>
       </c>
@@ -2483,7 +2499,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>43591.521164178237</v>
       </c>
@@ -2494,7 +2510,7 @@
         <v>43591</v>
       </c>
       <c r="D15" s="9">
-        <v>1.3194444443797693E-2</v>
+        <v>0.5131944444444444</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>26</v>
@@ -2515,7 +2531,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>43591.527513136578</v>
       </c>
@@ -2547,7 +2563,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>43591.537957824075</v>
       </c>
@@ -2579,7 +2595,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>43591.548731967589</v>
       </c>
@@ -2611,7 +2627,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>43591.560089768522</v>
       </c>
@@ -2643,7 +2659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>43591.572355104166</v>
       </c>
@@ -2672,7 +2688,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>43591.577724270828</v>
       </c>
@@ -2704,7 +2720,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>43591.58141392361</v>
       </c>
@@ -2736,7 +2752,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>43591.583598541663</v>
       </c>
@@ -2768,7 +2784,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>43591.6724153588</v>
       </c>
@@ -2791,7 +2807,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>43591.674202650465</v>
       </c>
@@ -2814,7 +2830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>43591.704277094905</v>
       </c>
@@ -2834,7 +2850,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>43591.755216921301</v>
       </c>
@@ -2854,7 +2870,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>43591.757524560184</v>
       </c>
@@ -2874,7 +2890,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>43591.775486631945</v>
       </c>
@@ -2894,7 +2910,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>43591.776427210643</v>
       </c>
@@ -2917,7 +2933,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>43592.481644421292</v>
       </c>
@@ -2946,7 +2962,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>43592.482017627313</v>
       </c>
@@ -2975,7 +2991,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>43592.50501202546</v>
       </c>
@@ -3007,7 +3023,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>43592.532280358791</v>
       </c>
@@ -3039,7 +3055,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>43592.545401550931</v>
       </c>
@@ -3080,7 +3096,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>43592.637291597217</v>
       </c>
@@ -3112,7 +3128,7 @@
         <v>14200</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>43592.563986909721</v>
       </c>
@@ -3156,7 +3172,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>43592.580991099538</v>
       </c>
@@ -3188,7 +3204,7 @@
         <v>3100</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>43592.581140219903</v>
       </c>
@@ -3232,7 +3248,7 @@
         <v>4480</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <v>43592.640366712963</v>
       </c>
@@ -3264,7 +3280,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>43592.657211875005</v>
       </c>
@@ -3296,7 +3312,7 @@
         <v>4090</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>43592.681611643522</v>
       </c>
@@ -3323,7 +3339,7 @@
       </c>
       <c r="J42" s="5"/>
     </row>
-    <row r="43" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>43592.691540694446</v>
       </c>
@@ -3367,7 +3383,7 @@
         <v>2375</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>43592.702423842595</v>
       </c>
@@ -3411,7 +3427,7 @@
         <v>1560</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <v>43593.43748443287</v>
       </c>
@@ -3443,7 +3459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>43593.44123866898</v>
       </c>
@@ -3472,7 +3488,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>43593.460052071758</v>
       </c>
@@ -3516,7 +3532,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
         <v>43593.476238275463</v>
       </c>
@@ -3560,7 +3576,7 @@
         <v>1740</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>43593.518983738424</v>
       </c>
@@ -3604,7 +3620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <v>43593.527186284722</v>
       </c>
@@ -3633,7 +3649,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>43593.548600451388</v>
       </c>
@@ -3662,7 +3678,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <v>43593.553772789353</v>
       </c>
@@ -3706,7 +3722,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
         <v>43593.598725358795</v>
       </c>
@@ -3729,7 +3745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <v>43593.610852187499</v>
       </c>
@@ -3770,7 +3786,7 @@
         <v>6250</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <v>43593.612856157408</v>
       </c>
@@ -3811,7 +3827,7 @@
         <v>7580</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
         <v>43593.617690162035</v>
       </c>
@@ -3852,7 +3868,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="57" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
         <v>43593.618488009262</v>
       </c>
@@ -3875,7 +3891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
         <v>43593.619830208336</v>
       </c>
@@ -3916,7 +3932,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
         <v>43593.656584456017</v>
       </c>
@@ -3957,7 +3973,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="60" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
         <v>43593.658092847225</v>
       </c>
@@ -4001,7 +4017,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="61" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A61" s="7">
         <v>43593.660192870375</v>
       </c>
@@ -4045,7 +4061,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
         <v>43593.6652215625</v>
       </c>
@@ -4089,7 +4105,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
         <v>43593.691000405088</v>
       </c>
@@ -4109,7 +4125,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
         <v>43594.407145740741</v>
       </c>
@@ -4153,7 +4169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A65" s="7">
         <v>43594.410411932869</v>
       </c>
@@ -4197,7 +4213,7 @@
         <v>2170</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A66" s="7">
         <v>43594.419389386574</v>
       </c>
@@ -4241,7 +4257,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <v>43594.424918101853</v>
       </c>
@@ -4285,7 +4301,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A68" s="7">
         <v>43594.431594340276</v>
       </c>
@@ -4317,7 +4333,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A69" s="7">
         <v>43594.432673472227</v>
       </c>
@@ -4361,7 +4377,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A70" s="7">
         <v>43594.435762604167</v>
       </c>
@@ -4405,7 +4421,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A71" s="7">
         <v>43594.444414444442</v>
       </c>
@@ -4449,7 +4465,7 @@
         <v>2460</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A72" s="7">
         <v>43594.445713379631</v>
       </c>
@@ -4481,7 +4497,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A73" s="7">
         <v>43594.461393437501</v>
       </c>
@@ -4513,7 +4529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A74" s="7">
         <v>43594.467428356482</v>
       </c>
@@ -4557,7 +4573,7 @@
         <v>5570</v>
       </c>
     </row>
-    <row r="75" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A75" s="7">
         <v>43594.491857604167</v>
       </c>
@@ -4601,7 +4617,7 @@
         <v>4680</v>
       </c>
     </row>
-    <row r="76" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A76" s="7">
         <v>43594.514163171298</v>
       </c>
@@ -4626,8 +4642,14 @@
       <c r="H76" s="5">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="77" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J76">
+        <v>60</v>
+      </c>
+      <c r="K76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A77" s="7">
         <v>43594.530017488425</v>
       </c>
@@ -4638,7 +4660,7 @@
         <v>43594</v>
       </c>
       <c r="D77" s="9">
-        <v>2.7777777781011537E-2</v>
+        <v>0.52777777777777779</v>
       </c>
       <c r="E77" s="5" t="s">
         <v>26</v>
@@ -4671,7 +4693,7 @@
         <v>2670</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A78" s="7">
         <v>43594.584730694449</v>
       </c>
@@ -4694,7 +4716,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A79" s="7">
         <v>43594.611498634258</v>
       </c>
@@ -4720,7 +4742,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A80" s="7">
         <v>43594.624838090276</v>
       </c>
@@ -4764,7 +4786,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A81" s="7">
         <v>43594.648807557867</v>
       </c>
@@ -4808,7 +4830,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="82" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A82" s="7">
         <v>43594.653585208333</v>
       </c>
@@ -4830,8 +4852,14 @@
       <c r="H82" s="5">
         <v>-2.6</v>
       </c>
-    </row>
-    <row r="83" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J82">
+        <v>60</v>
+      </c>
+      <c r="K82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A83" s="7">
         <v>43594.667883368056</v>
       </c>
@@ -4857,7 +4885,7 @@
         <v>-1.4</v>
       </c>
     </row>
-    <row r="84" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A84" s="7">
         <v>43594.676933946757</v>
       </c>
@@ -4877,7 +4905,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="85" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A85" s="7">
         <v>43594.68904351852</v>
       </c>
@@ -4921,7 +4949,7 @@
         <v>3890</v>
       </c>
     </row>
-    <row r="86" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A86" s="7">
         <v>43594.893515358795</v>
       </c>
@@ -4965,7 +4993,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="87" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A87" s="7">
         <v>43594.895805115739</v>
       </c>
@@ -5009,7 +5037,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="88" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A88" s="7">
         <v>43594.896885995375</v>
       </c>
@@ -5053,7 +5081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A89" s="7">
         <v>43594.89877886574</v>
       </c>
@@ -5097,7 +5125,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="90" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A90" s="7">
         <v>43594.900322071757</v>
       </c>
@@ -5138,7 +5166,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="91" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A91" s="7">
         <v>43594.901593657407</v>
       </c>
@@ -5179,7 +5207,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="92" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A92" s="7">
         <v>43594.903644548613</v>
       </c>
@@ -5220,7 +5248,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="93" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A93" s="7">
         <v>43594.905283796295</v>
       </c>
@@ -5261,7 +5289,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="94" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A94" s="7">
         <v>43594.907106331018</v>
       </c>
@@ -5305,7 +5333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A95" s="7">
         <v>43594.908273356486</v>
       </c>
@@ -5346,7 +5374,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="96" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A96" s="7">
         <v>43594.909638333338</v>
       </c>
@@ -5387,7 +5415,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="97" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A97" s="7">
         <v>43594.91069650463</v>
       </c>
@@ -5428,7 +5456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A98" s="7">
         <v>43594.912148344913</v>
       </c>
@@ -5469,7 +5497,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="99" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A99" s="7">
         <v>43594.913895949074</v>
       </c>
@@ -5510,7 +5538,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="100" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A100" s="7">
         <v>43595.442240902776</v>
       </c>
@@ -5530,7 +5558,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="101" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A101" s="7">
         <v>43595.448872152774</v>
       </c>
@@ -5571,7 +5599,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="102" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A102" s="7">
         <v>43595.470052662036</v>
       </c>
@@ -5606,7 +5634,7 @@
         <v>6300</v>
       </c>
     </row>
-    <row r="103" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A103" s="7">
         <v>43595.470242951385</v>
       </c>
@@ -5632,7 +5660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A104" s="7">
         <v>43595.472295949075</v>
       </c>
@@ -5676,7 +5704,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="105" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A105" s="7">
         <v>43595.474870532409</v>
       </c>
@@ -5720,7 +5748,7 @@
         <v>2980</v>
       </c>
     </row>
-    <row r="106" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A106" s="7">
         <v>43595.481380717596</v>
       </c>
@@ -5755,7 +5783,7 @@
         <v>7030</v>
       </c>
     </row>
-    <row r="107" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A107" s="7">
         <v>43595.490416296292</v>
       </c>
@@ -5796,7 +5824,7 @@
         <v>6300</v>
       </c>
     </row>
-    <row r="108" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A108" s="7">
         <v>43595.500877777777</v>
       </c>
@@ -5834,7 +5862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A109" s="7">
         <v>43595.509428749996</v>
       </c>
@@ -5869,7 +5897,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="110" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A110" s="7">
         <v>43595.513097534727</v>
       </c>
@@ -5913,7 +5941,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="111" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A111" s="7">
         <v>43595.516432615739</v>
       </c>
@@ -5954,7 +5982,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="112" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A112" s="7">
         <v>43595.524782893517</v>
       </c>
@@ -5998,7 +6026,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="113" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A113" s="7">
         <v>43595.537118668981</v>
       </c>
@@ -6042,7 +6070,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="114" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A114" s="7">
         <v>43595.554605081023</v>
       </c>
@@ -6065,7 +6093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A115" s="7">
         <v>43595.554936168977</v>
       </c>
@@ -6088,7 +6116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A116" s="7">
         <v>43595.556602696757</v>
       </c>
@@ -6111,7 +6139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A117" s="7">
         <v>43595.5592850463</v>
       </c>
@@ -6134,7 +6162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A118" s="7">
         <v>43595.568305081018</v>
       </c>
@@ -6169,7 +6197,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="119" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A119" s="7">
         <v>43595.569374467595</v>
       </c>
@@ -6210,7 +6238,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="120" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A120" s="7">
         <v>43595.586062511575</v>
       </c>
@@ -6245,7 +6273,7 @@
         <v>2650</v>
       </c>
     </row>
-    <row r="121" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A121" s="7">
         <v>43595.587130358792</v>
       </c>
@@ -6280,7 +6308,7 @@
         <v>2430</v>
       </c>
     </row>
-    <row r="122" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A122" s="7">
         <v>43595.588972465281</v>
       </c>
@@ -6315,7 +6343,7 @@
         <v>2430</v>
       </c>
     </row>
-    <row r="123" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A123" s="7">
         <v>43595.590072256949</v>
       </c>
@@ -6350,7 +6378,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="124" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A124" s="7">
         <v>43595.594992129627</v>
       </c>
@@ -6394,7 +6422,7 @@
         <v>1230</v>
       </c>
     </row>
-    <row r="125" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A125" s="7">
         <v>43595.619344803243</v>
       </c>
@@ -6438,7 +6466,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="126" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A126" s="7">
         <v>43595.663596446757</v>
       </c>
@@ -6473,7 +6501,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="127" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A127" s="7">
         <v>43595.682554699073</v>
       </c>
@@ -6514,7 +6542,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="128" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A128" s="7">
         <v>43595.689118402777</v>
       </c>
@@ -6549,7 +6577,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="129" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A129" s="7">
         <v>43595.691901261569</v>
       </c>
@@ -6569,7 +6597,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="130" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A130" s="7">
         <v>43595.693264699075</v>
       </c>
@@ -6591,8 +6619,14 @@
       <c r="H130" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="131" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J130">
+        <v>60</v>
+      </c>
+      <c r="K130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A131" s="7">
         <v>43595.707292939813</v>
       </c>
@@ -6614,8 +6648,14 @@
       <c r="H131" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="132" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J131" s="24">
+        <v>60</v>
+      </c>
+      <c r="K131" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A132" s="7">
         <v>43595.708949965279</v>
       </c>
@@ -6637,8 +6677,14 @@
       <c r="H132" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J132">
+        <v>60</v>
+      </c>
+      <c r="K132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A133" s="7">
         <v>43595.711790578702</v>
       </c>
@@ -6660,8 +6706,14 @@
       <c r="H133" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J133">
+        <v>60</v>
+      </c>
+      <c r="K133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A134" s="7">
         <v>43595.725159085647</v>
       </c>
@@ -6684,7 +6736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A135" s="7">
         <v>43598.523171504625</v>
       </c>
@@ -6728,7 +6780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A136" s="7">
         <v>43598.531430370371</v>
       </c>
@@ -6772,7 +6824,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="137" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A137" s="7">
         <v>43598.538723784717</v>
       </c>
@@ -6816,7 +6868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A138" s="7">
         <v>43598.55321135417</v>
       </c>
@@ -6860,7 +6912,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="139" spans="1:15" s="11" customFormat="1" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15" s="11" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A139" s="10">
         <v>43598.558324872683</v>
       </c>
@@ -6889,7 +6941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A140" s="7">
         <v>43598.568272129633</v>
       </c>
@@ -6933,7 +6985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A141" s="7">
         <v>43598.660832187496</v>
       </c>
@@ -7009,7 +7061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A143" s="7">
         <v>43599.412810810187</v>
       </c>
@@ -7050,7 +7102,7 @@
         <v>3260</v>
       </c>
     </row>
-    <row r="144" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A144" s="7">
         <v>43599.427670717589</v>
       </c>
@@ -7094,7 +7146,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="145" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A145" s="7">
         <v>43599.433456574072</v>
       </c>
@@ -7138,7 +7190,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="146" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A146" s="7">
         <v>43599.459267349535</v>
       </c>
@@ -7182,7 +7234,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="147" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A147" s="7">
         <v>43599.470011574071</v>
       </c>
@@ -7226,7 +7278,7 @@
         <v>2520</v>
       </c>
     </row>
-    <row r="148" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A148" s="7">
         <v>43599.485035810183</v>
       </c>
@@ -7252,7 +7304,7 @@
         <v>16.8</v>
       </c>
     </row>
-    <row r="149" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A149" s="7">
         <v>43599.500831736106</v>
       </c>
@@ -7278,7 +7330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A150" s="7">
         <v>43599.518437384264</v>
       </c>
@@ -7303,8 +7355,14 @@
       <c r="H150" s="5">
         <v>-2.7</v>
       </c>
-    </row>
-    <row r="151" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J150">
+        <v>60</v>
+      </c>
+      <c r="K150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A151" s="7">
         <v>43599.539609108797</v>
       </c>
@@ -7348,7 +7406,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="152" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A152" s="7">
         <v>43599.569834490743</v>
       </c>
@@ -7392,7 +7450,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="153" spans="1:15" s="11" customFormat="1" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:15" s="11" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A153" s="10">
         <v>43599.624617476853</v>
       </c>
@@ -7421,7 +7479,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="154" spans="1:15" s="11" customFormat="1" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:15" s="11" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A154" s="10">
         <v>43599.639232141199</v>
       </c>
@@ -7453,7 +7511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A155" s="7">
         <v>43599.738793206023</v>
       </c>
@@ -7497,7 +7555,7 @@
         <v>2160</v>
       </c>
     </row>
-    <row r="156" spans="1:15" s="11" customFormat="1" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:15" s="11" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A156" s="10">
         <v>43600.422265266199</v>
       </c>
@@ -7529,7 +7587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A157" s="7">
         <v>43600.482206006942</v>
       </c>
@@ -7573,7 +7631,7 @@
         <v>3240</v>
       </c>
     </row>
-    <row r="158" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A158" s="7">
         <v>43600.493555451394</v>
       </c>
@@ -7605,7 +7663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A159" s="7">
         <v>43600.498960439814</v>
       </c>
@@ -7649,7 +7707,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="160" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A160" s="7">
         <v>43600.528849884256</v>
       </c>
@@ -7693,7 +7751,7 @@
         <v>1450</v>
       </c>
     </row>
-    <row r="161" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A161" s="7">
         <v>43600.601932974532</v>
       </c>
@@ -7737,7 +7795,7 @@
         <v>2190</v>
       </c>
     </row>
-    <row r="162" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A162" s="7">
         <v>43600.638289583338</v>
       </c>
@@ -7781,7 +7839,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="163" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A163" s="7">
         <v>43600.686218657407</v>
       </c>
@@ -7825,7 +7883,7 @@
         <v>9850</v>
       </c>
     </row>
-    <row r="164" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A164" s="7">
         <v>43600.725389861109</v>
       </c>
@@ -7904,7 +7962,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="166" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A166" s="7">
         <v>43601.40923740741</v>
       </c>
@@ -7927,7 +7985,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="167" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A167" s="7">
         <v>43601.414449374999</v>
       </c>
@@ -7950,7 +8008,7 @@
         <v>-1.3</v>
       </c>
     </row>
-    <row r="168" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A168" s="7">
         <v>43601.415471493056</v>
       </c>
@@ -7979,7 +8037,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="169" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A169" s="7">
         <v>43601.417819421295</v>
       </c>
@@ -8008,7 +8066,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="170" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A170" s="7">
         <v>43601.419731273148</v>
       </c>
@@ -8037,7 +8095,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="171" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A171" s="7">
         <v>43601.427588611114</v>
       </c>
@@ -8066,7 +8124,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="172" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A172" s="7">
         <v>43602.442062349539</v>
       </c>
@@ -8139,7 +8197,7 @@
         <v>1190</v>
       </c>
     </row>
-    <row r="174" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A174" s="7">
         <v>43602.47989505787</v>
       </c>
@@ -8165,7 +8223,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="175" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A175" s="7">
         <v>43602.489967141199</v>
       </c>
@@ -8203,7 +8261,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="176" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A176" s="7">
         <v>43602.509337268522</v>
       </c>
@@ -8241,7 +8299,7 @@
         <v>3700</v>
       </c>
     </row>
-    <row r="177" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A177" s="7">
         <v>43602.522517500001</v>
       </c>
@@ -8276,7 +8334,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="178" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A178" s="7">
         <v>43606.707793877315</v>
       </c>
@@ -8317,7 +8375,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="179" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A179" s="7">
         <v>43606.723546145833</v>
       </c>
@@ -8358,7 +8416,7 @@
         <v>1830</v>
       </c>
     </row>
-    <row r="180" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A180" s="7">
         <v>43608.481453252316</v>
       </c>
@@ -8387,7 +8445,7 @@
         <v>9100</v>
       </c>
     </row>
-    <row r="181" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A181" s="7">
         <v>43608.482445162037</v>
       </c>
@@ -8416,7 +8474,7 @@
         <v>8050</v>
       </c>
     </row>
-    <row r="182" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A182" s="7">
         <v>43608.483487696758</v>
       </c>
@@ -8445,7 +8503,7 @@
         <v>7240</v>
       </c>
     </row>
-    <row r="183" spans="1:15" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="7">
         <v>43608.526771817131</v>
       </c>
@@ -8477,7 +8535,7 @@
         <v>3480</v>
       </c>
     </row>
-    <row r="184" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A184" s="7">
         <v>43619.387044270828</v>
       </c>
@@ -8500,7 +8558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A185" s="7">
         <v>43619.417066539347</v>
       </c>
@@ -8529,7 +8587,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="186" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A186" s="7">
         <v>43619.424325891203</v>
       </c>
@@ -8564,7 +8622,7 @@
         <v>8600</v>
       </c>
     </row>
-    <row r="187" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A187" s="7">
         <v>43619.430370590278</v>
       </c>
@@ -8593,7 +8651,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="188" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A188" s="7">
         <v>43619.448148344905</v>
       </c>
@@ -8616,7 +8674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A189" s="7">
         <v>43619.449386782406</v>
       </c>
@@ -8660,7 +8718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A190" s="7">
         <v>43619.457925891205</v>
       </c>
@@ -8704,7 +8762,7 @@
         <v>4910</v>
       </c>
     </row>
-    <row r="191" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A191" s="7">
         <v>43619.481042361112</v>
       </c>
@@ -8726,8 +8784,14 @@
       <c r="H191" s="5">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="192" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J191" s="5">
+        <v>60</v>
+      </c>
+      <c r="K191" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A192" s="7">
         <v>43619.482240219906</v>
       </c>
@@ -8756,7 +8820,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="193" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A193" s="7">
         <v>43619.485708449072</v>
       </c>
@@ -8785,7 +8849,7 @@
         <v>2470</v>
       </c>
     </row>
-    <row r="194" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A194" s="7">
         <v>43619.502512523148</v>
       </c>
@@ -8814,7 +8878,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="195" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A195" s="7">
         <v>43619.50333712963</v>
       </c>
@@ -8837,7 +8901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A196" s="7">
         <v>43619.512569479164</v>
       </c>
@@ -8859,8 +8923,14 @@
       <c r="H196" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="197" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J196" s="24">
+        <v>60</v>
+      </c>
+      <c r="K196" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A197" s="7">
         <v>43619.559027557872</v>
       </c>
@@ -8882,8 +8952,14 @@
       <c r="H197" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="198" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J197" s="5">
+        <v>60</v>
+      </c>
+      <c r="K197" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A198" s="7">
         <v>43619.560911979162</v>
       </c>
@@ -8906,7 +8982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A199" s="7">
         <v>43619.580106157402</v>
       </c>
@@ -8935,7 +9011,7 @@
         <v>8500</v>
       </c>
     </row>
-    <row r="200" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A200" s="7">
         <v>43619.586162476851</v>
       </c>
@@ -8958,7 +9034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A201" s="7">
         <v>43619.593100185186</v>
       </c>
@@ -8990,7 +9066,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="202" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A202" s="7">
         <v>43619.603138240738</v>
       </c>
@@ -9019,7 +9095,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="203" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A203" s="7">
         <v>43619.624149479168</v>
       </c>
@@ -9048,7 +9124,7 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="204" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A204" s="7">
         <v>43619.636075578703</v>
       </c>
@@ -9080,7 +9156,7 @@
         <v>2820</v>
       </c>
     </row>
-    <row r="205" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A205" s="7">
         <v>43619.657319212958</v>
       </c>
@@ -9112,7 +9188,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="206" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A206" s="7">
         <v>43619.669281388888</v>
       </c>
@@ -9135,7 +9211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A207" s="7">
         <v>43619.683368090278</v>
       </c>
@@ -9167,7 +9243,7 @@
         <v>2220</v>
       </c>
     </row>
-    <row r="208" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A208" s="7">
         <v>43620.42668315972</v>
       </c>
@@ -9193,7 +9269,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="209" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A209" s="7">
         <v>43620.433715914347</v>
       </c>
@@ -9222,7 +9298,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="210" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A210" s="7">
         <v>43620.449795451394</v>
       </c>
@@ -9251,7 +9327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A211" s="7">
         <v>43620.468617280094</v>
       </c>
@@ -9295,7 +9371,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="212" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A212" s="7">
         <v>43620.486011516201</v>
       </c>
@@ -9336,7 +9412,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="213" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A213" s="7">
         <v>43620.487928645831</v>
       </c>
@@ -9365,7 +9441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A214" s="7">
         <v>43620.488378425929</v>
       </c>
@@ -9385,7 +9461,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="215" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A215" s="7">
         <v>43620.488762453708</v>
       </c>
@@ -9405,7 +9481,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="216" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A216" s="7">
         <v>43620.502757766204</v>
       </c>
@@ -9475,7 +9551,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="218" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A218" s="7">
         <v>43620.516394976847</v>
       </c>
@@ -9501,7 +9577,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="219" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A219" s="7">
         <v>43620.531383842594</v>
       </c>
@@ -9524,7 +9600,7 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="220" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A220" s="7">
         <v>43620.534318229169</v>
       </c>
@@ -9553,7 +9629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A221" s="7">
         <v>43620.53862825231</v>
       </c>
@@ -9582,7 +9658,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="222" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A222" s="7">
         <v>43620.544621446759</v>
       </c>
@@ -9604,8 +9680,14 @@
       <c r="H222" s="5">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="223" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J222">
+        <v>60</v>
+      </c>
+      <c r="K222">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A223" s="7">
         <v>43620.559045000002</v>
       </c>
@@ -9646,7 +9728,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="224" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A224" s="7">
         <v>43620.562107916667</v>
       </c>
@@ -9669,7 +9751,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="225" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A225" s="7">
         <v>43620.57524528935</v>
       </c>
@@ -9710,7 +9792,7 @@
         <v>1540</v>
       </c>
     </row>
-    <row r="226" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A226" s="7">
         <v>43620.57848960648</v>
       </c>
@@ -9739,7 +9821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A227" s="7">
         <v>43620.589187465273</v>
       </c>
@@ -9762,7 +9844,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="228" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A228" s="7">
         <v>43620.646162557867</v>
       </c>
@@ -9803,7 +9885,7 @@
         <v>2215</v>
       </c>
     </row>
-    <row r="229" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A229" s="7">
         <v>43620.686772013883</v>
       </c>
@@ -9826,7 +9908,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="230" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A230" s="7">
         <v>43623.521720659723</v>
       </c>
@@ -9849,7 +9931,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="231" spans="1:15" s="22" customFormat="1" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:15" s="22" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A231" s="18">
         <v>43623.522309618056</v>
       </c>
@@ -9872,7 +9954,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="232" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A232" s="7">
         <v>43633.40398304398</v>
       </c>
@@ -9901,7 +9983,7 @@
         <v>5100</v>
       </c>
     </row>
-    <row r="233" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A233" s="7">
         <v>43633.416756932871</v>
       </c>
@@ -9930,7 +10012,7 @@
         <v>5100</v>
       </c>
     </row>
-    <row r="234" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A234" s="7">
         <v>43633.420208194446</v>
       </c>
@@ -9959,7 +10041,7 @@
         <v>14250</v>
       </c>
     </row>
-    <row r="235" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A235" s="7">
         <v>43633.428534791667</v>
       </c>
@@ -9988,7 +10070,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="236" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A236" s="7">
         <v>43633.4461915625</v>
       </c>
@@ -10017,7 +10099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A237" s="7">
         <v>43633.46175555556</v>
       </c>
@@ -10061,7 +10143,7 @@
         <v>2270</v>
       </c>
     </row>
-    <row r="238" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A238" s="7">
         <v>43633.50244113426</v>
       </c>
@@ -10090,7 +10172,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="239" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A239" s="7">
         <v>43633.504802060183</v>
       </c>
@@ -10119,7 +10201,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="240" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A240" s="7">
         <v>43633.523931469907</v>
       </c>
@@ -10142,13 +10224,13 @@
         <v>0</v>
       </c>
       <c r="J240" s="5">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="K240" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A241" s="7">
         <v>43633.530496736115</v>
       </c>
@@ -10192,7 +10274,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="242" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A242" s="7">
         <v>43633.533061898153</v>
       </c>
@@ -10221,7 +10303,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="243" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A243" s="7">
         <v>43633.539491469906</v>
       </c>
@@ -10250,7 +10332,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="244" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A244" s="7">
         <v>43633.543584953703</v>
       </c>
@@ -10279,7 +10361,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="245" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A245" s="7">
         <v>43633.547313564814</v>
       </c>
@@ -10308,7 +10390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A246" s="7">
         <v>43633.551025127315</v>
       </c>
@@ -10337,7 +10419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A247" s="7">
         <v>43633.562344479171</v>
       </c>
@@ -10366,7 +10448,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="248" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A248" s="7">
         <v>43633.590683958333</v>
       </c>
@@ -10410,7 +10492,7 @@
         <v>9400</v>
       </c>
     </row>
-    <row r="249" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A249" s="7">
         <v>43633.581785532406</v>
       </c>
@@ -10439,7 +10521,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="250" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A250" s="7">
         <v>43633.625512199069</v>
       </c>
@@ -10465,7 +10547,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="251" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A251" s="7">
         <v>43633.627015150458</v>
       </c>
@@ -10494,7 +10576,7 @@
         <v>7400</v>
       </c>
     </row>
-    <row r="252" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A252" s="7">
         <v>43633.63865868056</v>
       </c>
@@ -10526,7 +10608,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="253" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A253" s="7">
         <v>43633.660197569443</v>
       </c>
@@ -10558,7 +10640,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="254" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A254" s="7">
         <v>43633.689922777776</v>
       </c>
@@ -10590,7 +10672,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="255" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A255" s="7">
         <v>43634.393672152779</v>
       </c>
@@ -10619,7 +10701,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="256" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A256" s="7">
         <v>43634.396875138889</v>
       </c>
@@ -10648,7 +10730,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="257" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A257" s="7">
         <v>43634.405545023154</v>
       </c>
@@ -10671,13 +10753,13 @@
         <v>0</v>
       </c>
       <c r="J257" s="5">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="K257" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A258" s="7">
         <v>43634.416232280091</v>
       </c>
@@ -10706,7 +10788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A259" s="7">
         <v>43634.420364861115</v>
       </c>
@@ -10735,7 +10817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A260" s="7">
         <v>43634.424504351853</v>
       </c>
@@ -10779,7 +10861,7 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="261" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A261" s="7">
         <v>43634.427363206021</v>
       </c>
@@ -10808,7 +10890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A262" s="7">
         <v>43634.437920937504</v>
       </c>
@@ -10837,7 +10919,7 @@
         <v>7250</v>
       </c>
     </row>
-    <row r="263" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A263" s="7">
         <v>43634.446620960647</v>
       </c>
@@ -10866,7 +10948,7 @@
         <v>9500</v>
       </c>
     </row>
-    <row r="264" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A264" s="7">
         <v>43634.454626250001</v>
       </c>
@@ -10889,13 +10971,13 @@
         <v>0</v>
       </c>
       <c r="J264" s="5">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="K264" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A265" s="7">
         <v>43634.456643518519</v>
       </c>
@@ -10927,7 +11009,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="266" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A266" s="7">
         <v>43634.458449259255</v>
       </c>
@@ -10956,7 +11038,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="267" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A267" s="7">
         <v>43634.469420011577</v>
       </c>
@@ -10979,13 +11061,13 @@
         <v>0</v>
       </c>
       <c r="J267" s="5">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="K267" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A268" s="7">
         <v>43634.472232048611</v>
       </c>
@@ -11014,7 +11096,7 @@
         <v>3400</v>
       </c>
     </row>
-    <row r="269" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A269" s="7">
         <v>43634.478026145836</v>
       </c>
@@ -11043,7 +11125,7 @@
         <v>3150</v>
       </c>
     </row>
-    <row r="270" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A270" s="7">
         <v>43634.478377719905</v>
       </c>
@@ -11072,7 +11154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A271" s="7">
         <v>43634.486881469908</v>
       </c>
@@ -11101,7 +11183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A272" s="7">
         <v>43634.488325983795</v>
       </c>
@@ -11130,7 +11212,7 @@
         <v>8100</v>
       </c>
     </row>
-    <row r="273" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A273" s="7">
         <v>43634.496477800931</v>
       </c>
@@ -11162,7 +11244,7 @@
         <v>8100</v>
       </c>
     </row>
-    <row r="274" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A274" s="7">
         <v>43634.500037627316</v>
       </c>
@@ -11191,7 +11273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A275" s="7">
         <v>43634.503317557872</v>
       </c>
@@ -11220,7 +11302,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="276" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A276" s="7">
         <v>43634.5105887963</v>
       </c>
@@ -11243,13 +11325,13 @@
         <v>0</v>
       </c>
       <c r="J276" s="5">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="K276" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A277" s="7">
         <v>43634.51392675926</v>
       </c>
@@ -11260,7 +11342,7 @@
         <v>43634</v>
       </c>
       <c r="D277" s="9">
-        <v>1.0416666664241347E-2</v>
+        <v>0.51041666666666663</v>
       </c>
       <c r="E277" s="5" t="s">
         <v>26</v>
@@ -11281,7 +11363,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="278" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A278" s="7">
         <v>43634.530469999998</v>
       </c>
@@ -11292,7 +11374,7 @@
         <v>43634</v>
       </c>
       <c r="D278" s="9">
-        <v>2.7777777781011537E-2</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="E278" s="5" t="s">
         <v>26</v>
@@ -11310,7 +11392,7 @@
         <v>1760</v>
       </c>
     </row>
-    <row r="279" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A279" s="7">
         <v>43634.56578636574</v>
       </c>
@@ -11400,7 +11482,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="282" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A282" s="7">
         <v>43634.633482164354</v>
       </c>
@@ -11429,7 +11511,7 @@
         <v>5100</v>
       </c>
     </row>
-    <row r="283" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A283" s="7">
         <v>43637.422400451389</v>
       </c>
@@ -11458,7 +11540,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="284" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A284" s="7">
         <v>43641.40604130787</v>
       </c>
@@ -11499,7 +11581,7 @@
         <v>3015</v>
       </c>
     </row>
-    <row r="285" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A285" s="7">
         <v>43641.415160428238</v>
       </c>
@@ -11540,7 +11622,7 @@
         <v>2750</v>
       </c>
     </row>
-    <row r="286" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A286" s="7">
         <v>43641.438067060182</v>
       </c>
@@ -11581,7 +11663,7 @@
         <v>2620</v>
       </c>
     </row>
-    <row r="287" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A287" s="7">
         <v>43641.454948587962</v>
       </c>
@@ -11622,7 +11704,7 @@
         <v>2475</v>
       </c>
     </row>
-    <row r="288" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A288" s="7">
         <v>43641.468790266204</v>
       </c>
@@ -11663,7 +11745,7 @@
         <v>2640</v>
       </c>
     </row>
-    <row r="289" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A289" s="7">
         <v>43641.543771076387</v>
       </c>
@@ -11704,7 +11786,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="290" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A290" s="7">
         <v>43641.555053761578</v>
       </c>
@@ -11745,7 +11827,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="291" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A291" s="7">
         <v>43641.635631805555</v>
       </c>
@@ -11786,7 +11868,7 @@
         <v>1815</v>
       </c>
     </row>
-    <row r="292" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A292" s="7">
         <v>43641.647440000001</v>
       </c>
@@ -11827,7 +11909,7 @@
         <v>1565</v>
       </c>
     </row>
-    <row r="293" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A293" s="7">
         <v>43641.6602040625</v>
       </c>
@@ -11868,7 +11950,7 @@
         <v>1645</v>
       </c>
     </row>
-    <row r="294" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A294" s="7">
         <v>43641.689663888887</v>
       </c>
@@ -11909,7 +11991,7 @@
         <v>1730</v>
       </c>
     </row>
-    <row r="295" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A295" s="7">
         <v>43641.701291400459</v>
       </c>
@@ -11950,7 +12032,7 @@
         <v>1930</v>
       </c>
     </row>
-    <row r="296" spans="1:17" s="22" customFormat="1" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:17" s="22" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A296" s="18">
         <v>43641.717524178239</v>
       </c>
@@ -11994,7 +12076,7 @@
         <v>2120</v>
       </c>
     </row>
-    <row r="297" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A297" s="7">
         <v>43647.378567395834</v>
       </c>
@@ -12027,7 +12109,7 @@
       </c>
       <c r="Q297" s="5"/>
     </row>
-    <row r="298" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A298" s="7">
         <v>43647.39412060185</v>
       </c>
@@ -12060,7 +12142,7 @@
       </c>
       <c r="Q298" s="5"/>
     </row>
-    <row r="299" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A299" s="7">
         <v>43647.403549803239</v>
       </c>
@@ -12093,7 +12175,7 @@
       </c>
       <c r="Q299" s="5"/>
     </row>
-    <row r="300" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A300" s="7">
         <v>43647.418112916668</v>
       </c>
@@ -12126,7 +12208,7 @@
       </c>
       <c r="Q300" s="5"/>
     </row>
-    <row r="301" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A301" s="7">
         <v>43647.437997430556</v>
       </c>
@@ -12158,7 +12240,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="302" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A302" s="7">
         <v>43647.442859641204</v>
       </c>
@@ -12191,7 +12273,7 @@
       </c>
       <c r="Q302" s="5"/>
     </row>
-    <row r="303" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A303" s="7">
         <v>43647.44526699074</v>
       </c>
@@ -12214,7 +12296,7 @@
         <v>0</v>
       </c>
       <c r="J303" s="5">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="K303" s="5">
         <v>0</v>
@@ -12224,7 +12306,7 @@
       </c>
       <c r="Q303" s="5"/>
     </row>
-    <row r="304" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A304" s="7">
         <v>43647.445862928245</v>
       </c>
@@ -12257,7 +12339,7 @@
       </c>
       <c r="Q304" s="5"/>
     </row>
-    <row r="305" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A305" s="7">
         <v>43647.452365173609</v>
       </c>
@@ -12290,7 +12372,7 @@
       </c>
       <c r="Q305" s="5"/>
     </row>
-    <row r="306" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A306" s="7">
         <v>43647.46204752315</v>
       </c>
@@ -12313,7 +12395,7 @@
         <v>0</v>
       </c>
       <c r="J306" s="5">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="K306" s="5">
         <v>0</v>
@@ -12323,7 +12405,7 @@
       </c>
       <c r="Q306" s="5"/>
     </row>
-    <row r="307" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A307" s="7">
         <v>43647.47148359954</v>
       </c>
@@ -12356,7 +12438,7 @@
       </c>
       <c r="Q307" s="5"/>
     </row>
-    <row r="308" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A308" s="7">
         <v>43647.475172638893</v>
       </c>
@@ -12389,7 +12471,7 @@
       </c>
       <c r="Q308" s="5"/>
     </row>
-    <row r="309" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A309" s="7">
         <v>43647.482570231485</v>
       </c>
@@ -12412,7 +12494,7 @@
         <v>0</v>
       </c>
       <c r="J309" s="5">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="K309" s="5">
         <v>0</v>
@@ -12422,7 +12504,7 @@
       </c>
       <c r="Q309" s="5"/>
     </row>
-    <row r="310" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A310" s="7">
         <v>43647.489491956017</v>
       </c>
@@ -12455,7 +12537,7 @@
       </c>
       <c r="Q310" s="5"/>
     </row>
-    <row r="311" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A311" s="7">
         <v>43647.495944016206</v>
       </c>
@@ -12488,7 +12570,7 @@
       </c>
       <c r="Q311" s="5"/>
     </row>
-    <row r="312" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A312" s="7">
         <v>43647.496494571758</v>
       </c>
@@ -12521,7 +12603,7 @@
       </c>
       <c r="Q312" s="5"/>
     </row>
-    <row r="313" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A313" s="7">
         <v>43647.5053858912</v>
       </c>
@@ -12554,7 +12636,7 @@
       </c>
       <c r="Q313" s="5"/>
     </row>
-    <row r="314" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A314" s="7">
         <v>43647.512554305555</v>
       </c>
@@ -12590,7 +12672,7 @@
       </c>
       <c r="Q314" s="5"/>
     </row>
-    <row r="315" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A315" s="7">
         <v>43647.513685578699</v>
       </c>
@@ -12623,7 +12705,7 @@
       </c>
       <c r="Q315" s="5"/>
     </row>
-    <row r="316" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A316" s="7">
         <v>43647.518523483799</v>
       </c>
@@ -12656,7 +12738,7 @@
       </c>
       <c r="Q316" s="5"/>
     </row>
-    <row r="317" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A317" s="7">
         <v>43647.519861805558</v>
       </c>
@@ -12692,7 +12774,7 @@
       </c>
       <c r="Q317" s="5"/>
     </row>
-    <row r="318" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A318" s="7">
         <v>43647.535344895834</v>
       </c>
@@ -12725,7 +12807,7 @@
       </c>
       <c r="Q318" s="5"/>
     </row>
-    <row r="319" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A319" s="7">
         <v>43647.537166388887</v>
       </c>
@@ -12758,7 +12840,7 @@
       </c>
       <c r="Q319" s="5"/>
     </row>
-    <row r="320" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A320" s="7">
         <v>43647.538050277777</v>
       </c>
@@ -12781,7 +12863,7 @@
         <v>0</v>
       </c>
       <c r="J320" s="5">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="K320" s="5">
         <v>0</v>
@@ -12791,7 +12873,7 @@
       </c>
       <c r="Q320" s="5"/>
     </row>
-    <row r="321" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A321" s="7">
         <v>43647.540616631944</v>
       </c>
@@ -12824,7 +12906,7 @@
       </c>
       <c r="Q321" s="5"/>
     </row>
-    <row r="322" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A322" s="7">
         <v>43647.54435773148</v>
       </c>
@@ -12857,7 +12939,7 @@
       </c>
       <c r="Q322" s="5"/>
     </row>
-    <row r="323" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A323" s="7">
         <v>43647.547887106484</v>
       </c>
@@ -12890,7 +12972,7 @@
       </c>
       <c r="Q323" s="5"/>
     </row>
-    <row r="324" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A324" s="7">
         <v>43647.551679976852</v>
       </c>
@@ -12923,7 +13005,7 @@
       </c>
       <c r="Q324" s="5"/>
     </row>
-    <row r="325" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A325" s="7">
         <v>43647.55485487268</v>
       </c>
@@ -12956,7 +13038,7 @@
       </c>
       <c r="Q325" s="5"/>
     </row>
-    <row r="326" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A326" s="7">
         <v>43647.586594768523</v>
       </c>
@@ -12992,7 +13074,7 @@
       </c>
       <c r="Q326" s="5"/>
     </row>
-    <row r="327" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A327" s="7">
         <v>43647.578063356486</v>
       </c>
@@ -13025,7 +13107,7 @@
       </c>
       <c r="Q327" s="5"/>
     </row>
-    <row r="328" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A328" s="7">
         <v>43647.581616527779</v>
       </c>
@@ -13061,7 +13143,7 @@
       </c>
       <c r="Q328" s="5"/>
     </row>
-    <row r="329" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A329" s="7">
         <v>43647.586999560182</v>
       </c>
@@ -13097,7 +13179,7 @@
       </c>
       <c r="Q329" s="5"/>
     </row>
-    <row r="330" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A330" s="7">
         <v>43647.587708356485</v>
       </c>
@@ -13130,7 +13212,7 @@
       </c>
       <c r="Q330" s="5"/>
     </row>
-    <row r="331" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A331" s="7">
         <v>43647.58930334491</v>
       </c>
@@ -13163,7 +13245,7 @@
       </c>
       <c r="Q331" s="5"/>
     </row>
-    <row r="332" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A332" s="7">
         <v>43647.614860520829</v>
       </c>
@@ -13196,7 +13278,7 @@
       </c>
       <c r="Q332" s="5"/>
     </row>
-    <row r="333" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A333" s="7">
         <v>43647.616616493055</v>
       </c>
@@ -13219,7 +13301,7 @@
         <v>0</v>
       </c>
       <c r="J333" s="5">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="K333" s="5">
         <v>0</v>
@@ -13229,7 +13311,7 @@
       </c>
       <c r="Q333" s="5"/>
     </row>
-    <row r="334" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A334" s="7">
         <v>43647.628458217594</v>
       </c>
@@ -13256,7 +13338,7 @@
       </c>
       <c r="Q334" s="5"/>
     </row>
-    <row r="335" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A335" s="7">
         <v>43647.648176006944</v>
       </c>
@@ -13289,7 +13371,7 @@
       </c>
       <c r="Q335" s="5"/>
     </row>
-    <row r="336" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A336" s="7">
         <v>43647.652004189818</v>
       </c>
@@ -13322,7 +13404,7 @@
       </c>
       <c r="Q336" s="5"/>
     </row>
-    <row r="337" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A337" s="7">
         <v>43647.663755868052</v>
       </c>
@@ -13355,7 +13437,7 @@
       </c>
       <c r="Q337" s="5"/>
     </row>
-    <row r="338" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A338" s="7">
         <v>43648.434577314816</v>
       </c>
@@ -13391,7 +13473,7 @@
       </c>
       <c r="Q338" s="5"/>
     </row>
-    <row r="339" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A339" s="7">
         <v>43648.464827615739</v>
       </c>
@@ -13424,7 +13506,7 @@
       </c>
       <c r="Q339" s="5"/>
     </row>
-    <row r="340" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A340" s="7">
         <v>43648.49087303241</v>
       </c>
@@ -13454,7 +13536,7 @@
       </c>
       <c r="Q340" s="5"/>
     </row>
-    <row r="341" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A341" s="7">
         <v>43648.505817361111</v>
       </c>
@@ -13487,7 +13569,7 @@
       </c>
       <c r="Q341" s="5"/>
     </row>
-    <row r="342" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A342" s="7">
         <v>43648.523454918977</v>
       </c>
@@ -13517,7 +13599,7 @@
       </c>
       <c r="Q342" s="5"/>
     </row>
-    <row r="343" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A343" s="7">
         <v>43648.535805590276</v>
       </c>
@@ -13528,7 +13610,7 @@
         <v>43648</v>
       </c>
       <c r="D343" s="9">
-        <v>0.54097222222480923</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="E343" s="5" t="s">
         <v>342</v>
@@ -13543,7 +13625,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="344" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A344" s="7">
         <v>43648.557352407406</v>
       </c>
@@ -13576,7 +13658,7 @@
       </c>
       <c r="Q344" s="5"/>
     </row>
-    <row r="345" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A345" s="7">
         <v>43648.574154016205</v>
       </c>
@@ -13612,7 +13694,7 @@
       </c>
       <c r="Q345" s="5"/>
     </row>
-    <row r="346" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A346" s="7">
         <v>43648.597286747681</v>
       </c>
@@ -13645,7 +13727,7 @@
       </c>
       <c r="Q346" s="5"/>
     </row>
-    <row r="347" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A347" s="7">
         <v>43648.600304039355</v>
       </c>
@@ -13714,7 +13796,7 @@
       </c>
       <c r="Q348" s="5"/>
     </row>
-    <row r="349" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A349" s="7">
         <v>43657.492113460648</v>
       </c>
@@ -13743,7 +13825,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="350" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A350" s="7">
         <v>43657.493938182874</v>
       </c>
@@ -13776,13 +13858,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U350">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="SDG-072"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:U350"/>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1"/>
     <hyperlink ref="G6" r:id="rId2"/>

</xml_diff>